<commit_message>
Add topics to mock data, and build interactive topic visualization
</commit_message>
<xml_diff>
--- a/data/mock-data.xlsx
+++ b/data/mock-data.xlsx
@@ -15,7 +15,7 @@
     <sheet name="mock-data" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="mock_data">'mock-data'!$A$2:$O$15</definedName>
+    <definedName name="mock_data">'mock-data'!$A$2:$AA$15</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -93,6 +93,42 @@
   </si>
   <si>
     <t>Truancy</t>
+  </si>
+  <si>
+    <t>Pregnant</t>
+  </si>
+  <si>
+    <t>Birth</t>
+  </si>
+  <si>
+    <t>Police</t>
+  </si>
+  <si>
+    <t>Protection Order</t>
+  </si>
+  <si>
+    <t>Opiates</t>
+  </si>
+  <si>
+    <t>Overdose</t>
+  </si>
+  <si>
+    <t>Suicide</t>
+  </si>
+  <si>
+    <t>Fatality</t>
+  </si>
+  <si>
+    <t>Medical Care</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Housing</t>
+  </si>
+  <si>
+    <t>Low Income</t>
   </si>
 </sst>
 </file>
@@ -758,11 +794,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="200743568"/>
-        <c:axId val="200744128"/>
+        <c:axId val="417500240"/>
+        <c:axId val="417500800"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="200743568"/>
+        <c:axId val="417500240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -819,12 +855,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200744128"/>
+        <c:crossAx val="417500800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="200744128"/>
+        <c:axId val="417500800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="200743568"/>
+        <c:crossAx val="417500240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1816,13 +1852,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="J3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N16" sqref="N16"/>
+      <selection pane="bottomRight" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1867,7 @@
     <col min="2" max="12" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
@@ -1859,8 +1895,20 @@
       </c>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
     </row>
-    <row r="2" spans="1:15" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -1906,8 +1954,44 @@
       <c r="O2" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="P2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="V2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="W2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="X2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1953,8 +2037,44 @@
       <c r="O3">
         <v>60</v>
       </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>20</v>
+      </c>
+      <c r="S3">
+        <v>20</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>0</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>40</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
@@ -2000,8 +2120,44 @@
       <c r="O4">
         <v>60</v>
       </c>
+      <c r="P4">
+        <v>10</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>10</v>
+      </c>
+      <c r="S4">
+        <v>15</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>20</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -2047,8 +2203,44 @@
       <c r="O5">
         <v>20</v>
       </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>10</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
+        <v>0</v>
+      </c>
+      <c r="Y5">
+        <v>50</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -2094,8 +2286,44 @@
       <c r="O6">
         <v>10</v>
       </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>50</v>
+      </c>
+      <c r="Z6">
+        <v>20</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -2141,8 +2369,44 @@
       <c r="O7">
         <v>10</v>
       </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>10</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>40</v>
+      </c>
+      <c r="Z7">
+        <v>30</v>
+      </c>
+      <c r="AA7">
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2188,8 +2452,44 @@
       <c r="O8">
         <v>0</v>
       </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>10</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>10</v>
+      </c>
+      <c r="U8">
+        <v>20</v>
+      </c>
+      <c r="V8">
+        <v>10</v>
+      </c>
+      <c r="W8">
+        <v>10</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>60</v>
+      </c>
+      <c r="Z8">
+        <v>40</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
@@ -2235,8 +2535,44 @@
       <c r="O9">
         <v>0</v>
       </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>20</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>20</v>
+      </c>
+      <c r="U9">
+        <v>10</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>5</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>40</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
@@ -2282,8 +2618,44 @@
       <c r="O10">
         <v>0</v>
       </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>20</v>
+      </c>
+      <c r="U10">
+        <v>5</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>35</v>
+      </c>
+      <c r="AA10">
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
@@ -2329,8 +2701,44 @@
       <c r="O11">
         <v>0</v>
       </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>10</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
+      <c r="X11">
+        <v>20</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>35</v>
+      </c>
+      <c r="AA11">
+        <v>15</v>
+      </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>1</v>
       </c>
@@ -2376,8 +2784,44 @@
       <c r="O12">
         <v>0</v>
       </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>10</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>0</v>
+      </c>
+      <c r="X12">
+        <v>10</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>20</v>
+      </c>
+      <c r="AA12">
+        <v>30</v>
+      </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
@@ -2423,8 +2867,44 @@
       <c r="O13">
         <v>0</v>
       </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>5</v>
+      </c>
+      <c r="U13">
+        <v>0</v>
+      </c>
+      <c r="V13">
+        <v>0</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>10</v>
+      </c>
+      <c r="AA13">
+        <v>40</v>
+      </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -2470,8 +2950,44 @@
       <c r="O14">
         <v>0</v>
       </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>0</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>30</v>
+      </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
@@ -2516,16 +3032,52 @@
       </c>
       <c r="O15">
         <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B17" s="3">
         <f t="shared" ref="B17" ca="1" si="0">B16+60+(RAND()-0.5)*20</f>
-        <v>54.111500149222238</v>
+        <v>63.069787702320063</v>
       </c>
       <c r="D17" s="5">
         <f t="shared" ref="D17" ca="1" si="1">IF(RAND()&lt;0.2, MAX(1, D16-1), IF(RAND()&lt;0.3, MIN(10, D16+1), D16))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="5">
         <f t="shared" ref="E17" ca="1" si="2">IF(RAND()&lt;0.2, MAX(1, E16-1), IF(RAND()&lt;0.3, MIN(10, E16+1), E16))</f>
@@ -2533,7 +3085,7 @@
       </c>
       <c r="F17" s="5">
         <f t="shared" ref="F17" ca="1" si="3">IF(RAND()&lt;0.2, MAX(1, F16-1), IF(RAND()&lt;0.3, MIN(10, F16+1), F16))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M17" t="s">
         <v>13</v>

</xml_diff>